<commit_message>
Parameters of different levels
</commit_message>
<xml_diff>
--- a/EldersAmbition/map/地图.xlsx
+++ b/EldersAmbition/map/地图.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1782" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="220">
   <si>
     <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -873,6 +873,30 @@
   </si>
   <si>
     <t>e_9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>伤害</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主角攻击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主角防御</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总经验</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总金钱</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1637,11 +1661,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -1652,11 +1676,10 @@
     <col min="4" max="4" width="6.19921875" customWidth="1"/>
     <col min="5" max="5" width="5.796875" customWidth="1"/>
     <col min="6" max="6" width="8.59765625" customWidth="1"/>
-    <col min="9" max="9" width="6.796875" customWidth="1"/>
-    <col min="10" max="10" width="5.69921875" customWidth="1"/>
+    <col min="12" max="12" width="6.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1675,8 +1698,26 @@
       <c r="F1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J1" t="s">
+        <v>218</v>
+      </c>
+      <c r="K1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M1" t="s">
+        <v>215</v>
+      </c>
+      <c r="N1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>50</v>
       </c>
@@ -1701,8 +1742,25 @@
       <c r="H2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <f>I2*E2</f>
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <f>I2*D2</f>
+        <v>5</v>
+      </c>
+      <c r="M2">
+        <v>820</v>
+      </c>
+      <c r="N2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>75</v>
       </c>
@@ -1727,8 +1785,19 @@
       <c r="H3" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J26" si="0">I3*E3</f>
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K26" si="1">I3*D3</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>100</v>
       </c>
@@ -1753,8 +1822,19 @@
       <c r="H4" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>15</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>110</v>
       </c>
@@ -1779,8 +1859,19 @@
       <c r="H5" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>200</v>
       </c>
@@ -1805,8 +1896,19 @@
       <c r="H6" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>150</v>
       </c>
@@ -1831,8 +1933,19 @@
       <c r="H7" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>125</v>
       </c>
@@ -1857,8 +1970,19 @@
       <c r="H8" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>150</v>
       </c>
@@ -1883,8 +2007,19 @@
       <c r="H9" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>9</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>300</v>
       </c>
@@ -1909,8 +2044,19 @@
       <c r="H10" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>400</v>
       </c>
@@ -1935,8 +2081,19 @@
       <c r="H11" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>500</v>
       </c>
@@ -1961,8 +2118,19 @@
       <c r="H12" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>250</v>
       </c>
@@ -1976,7 +2144,7 @@
         <v>20</v>
       </c>
       <c r="E13">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
         <v>56</v>
@@ -1987,22 +2155,33 @@
       <c r="H13" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>450</v>
       </c>
       <c r="B14">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="C14">
         <v>90</v>
       </c>
       <c r="D14">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E14">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F14" t="s">
         <v>57</v>
@@ -2013,22 +2192,37 @@
       <c r="H14" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14:L20" si="2">A14/($M$2-C14)*(B14-$N$2)</f>
+        <v>-363.69863013698631</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>550</v>
       </c>
       <c r="B15">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="C15">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D15">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E15">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F15" t="s">
         <v>58</v>
@@ -2039,19 +2233,34 @@
       <c r="H15" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>-435.41666666666663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>100</v>
+        <v>600</v>
       </c>
       <c r="B16">
-        <v>200</v>
+        <v>135</v>
       </c>
       <c r="C16">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D16">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E16">
         <v>25</v>
@@ -2065,22 +2274,37 @@
       <c r="H16" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>-474.12587412587413</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>700</v>
       </c>
       <c r="B17">
-        <v>210</v>
+        <v>140</v>
       </c>
       <c r="C17">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D17">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E17">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F17" t="s">
         <v>60</v>
@@ -2091,22 +2315,37 @@
       <c r="H17" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>-552.11267605633805</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1300</v>
       </c>
       <c r="B18">
-        <v>240</v>
+        <v>130</v>
       </c>
       <c r="C18">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D18">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="E18">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F18" t="s">
         <v>61</v>
@@ -2117,22 +2356,37 @@
       <c r="H18" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>7</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>154</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>154</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>-1043.661971830986</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>800</v>
       </c>
       <c r="B19">
+        <v>80</v>
+      </c>
+      <c r="C19">
         <v>60</v>
       </c>
-      <c r="C19">
-        <v>50</v>
-      </c>
       <c r="D19">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="E19">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -2143,22 +2397,37 @@
       <c r="H19" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="2"/>
+        <v>-652.63157894736844</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1200</v>
       </c>
       <c r="B20">
+        <v>160</v>
+      </c>
+      <c r="C20">
         <v>130</v>
       </c>
-      <c r="C20">
-        <v>90</v>
-      </c>
       <c r="D20">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="E20">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="F20">
         <v>2</v>
@@ -2169,8 +2438,23 @@
       <c r="H20" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>-939.13043478260863</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>600</v>
       </c>
@@ -2181,10 +2465,10 @@
         <v>15</v>
       </c>
       <c r="D21">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E21">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F21">
         <v>3</v>
@@ -2195,22 +2479,33 @@
       <c r="H21" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>900</v>
       </c>
       <c r="B22">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="C22">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="D22">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="E22">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="F22">
         <v>4</v>
@@ -2221,22 +2516,37 @@
       <c r="H22" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="L22">
+        <f t="shared" ref="L22:L28" si="3">A22/($M$2-C22)*(B22-$N$2)</f>
+        <v>-725</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>700</v>
       </c>
       <c r="B23">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C23">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D23">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="E23">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="F23">
         <v>5</v>
@@ -2247,22 +2557,37 @@
       <c r="H23" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="3"/>
+        <v>-578.0645161290322</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1100</v>
       </c>
       <c r="B24">
+        <v>150</v>
+      </c>
+      <c r="C24">
         <v>120</v>
       </c>
-      <c r="C24">
-        <v>80</v>
-      </c>
       <c r="D24">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="E24">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="F24">
         <v>6</v>
@@ -2273,22 +2598,37 @@
       <c r="H24" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="3"/>
+        <v>-864.28571428571422</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1000</v>
       </c>
       <c r="B25">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="C25">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="D25">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="E25">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="F25">
         <v>7</v>
@@ -2299,22 +2639,37 @@
       <c r="H25" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="3"/>
+        <v>-794.32624113475185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1300</v>
       </c>
       <c r="B26">
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="C26">
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="D26">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="E26">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F26">
         <v>8</v>
@@ -2325,13 +2680,28 @@
       <c r="H26" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="3"/>
+        <v>-975</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2500</v>
       </c>
       <c r="B27">
-        <v>600</v>
+        <v>650</v>
       </c>
       <c r="C27">
         <v>500</v>
@@ -2348,16 +2718,20 @@
       <c r="H27" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <f t="shared" si="3"/>
+        <v>-390.625</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3000</v>
       </c>
       <c r="B28">
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="C28">
-        <v>700</v>
+        <v>650</v>
       </c>
       <c r="D28">
         <v>250</v>
@@ -2371,8 +2745,32 @@
       <c r="H28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <f t="shared" si="3"/>
+        <v>882.35294117647061</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <f>SUM(J2:J26)</f>
+        <v>1149</v>
+      </c>
+      <c r="K30">
+        <f>SUM(K2:K26)</f>
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <f>J30/30*5</f>
+        <v>191.5</v>
+      </c>
+      <c r="K31">
+        <f>K30/25*4</f>
+        <v>198.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
         <v>173</v>
       </c>
@@ -2435,7 +2833,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -3026,7 +3424,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -3327,7 +3725,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3846,7 +4246,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -4250,10 +4650,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -4268,7 +4668,7 @@
     <col min="10" max="10" width="5.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -4287,704 +4687,996 @@
       <c r="F1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="I1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J1" t="s">
+        <v>218</v>
+      </c>
+      <c r="K1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>166</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <f>I2*E2</f>
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <f>I2*D2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>75</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J26" si="0">I3*E3</f>
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K26" si="1">I3*D3</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>169</v>
+      </c>
+      <c r="I4">
+        <v>15</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>110</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
+        <v>170</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>200</v>
+      </c>
+      <c r="B6">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" t="s">
+        <v>171</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>150</v>
+      </c>
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>172</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>125</v>
+      </c>
+      <c r="B8">
+        <v>40</v>
+      </c>
+      <c r="C8">
+        <v>28</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>150</v>
+      </c>
+      <c r="B9">
+        <v>52</v>
+      </c>
+      <c r="C9">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="4">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" t="s">
+        <v>185</v>
+      </c>
+      <c r="I9">
+        <v>9</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>300</v>
+      </c>
+      <c r="B10">
+        <v>60</v>
+      </c>
+      <c r="C10">
+        <v>36</v>
+      </c>
+      <c r="D10">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" t="s">
+        <v>183</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>400</v>
+      </c>
+      <c r="B11">
+        <v>72</v>
+      </c>
+      <c r="C11">
+        <v>40</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" t="s">
+        <v>181</v>
+      </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>500</v>
+      </c>
+      <c r="B12">
+        <v>92</v>
+      </c>
+      <c r="C12">
+        <v>52</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" t="s">
+        <v>189</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>250</v>
+      </c>
+      <c r="B13">
+        <v>96</v>
+      </c>
+      <c r="C13">
+        <v>56</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" t="s">
+        <v>182</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>450</v>
+      </c>
+      <c r="B14">
+        <v>88</v>
+      </c>
+      <c r="C14">
+        <v>72</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" t="s">
+        <v>184</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>550</v>
+      </c>
+      <c r="B15">
+        <v>104</v>
+      </c>
+      <c r="C15">
+        <v>80</v>
+      </c>
+      <c r="D15">
+        <v>22</v>
+      </c>
+      <c r="E15">
+        <v>22</v>
+      </c>
+      <c r="F15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" t="s">
+        <v>187</v>
+      </c>
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>600</v>
+      </c>
+      <c r="B16">
+        <v>108</v>
+      </c>
+      <c r="C16">
+        <v>84</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16">
+        <v>25</v>
+      </c>
+      <c r="F16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" t="s">
+        <v>190</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>700</v>
+      </c>
+      <c r="B17">
+        <v>112</v>
+      </c>
+      <c r="C17">
+        <v>88</v>
+      </c>
+      <c r="D17">
+        <v>28</v>
+      </c>
+      <c r="E17">
+        <v>28</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" t="s">
+        <v>188</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1300</v>
+      </c>
+      <c r="B18">
+        <v>104</v>
+      </c>
+      <c r="C18">
+        <v>88</v>
+      </c>
+      <c r="D18">
+        <v>22</v>
+      </c>
+      <c r="E18">
+        <v>22</v>
+      </c>
+      <c r="F18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" t="s">
+        <v>191</v>
+      </c>
+      <c r="I18">
+        <v>7</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>154</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>800</v>
+      </c>
+      <c r="B19">
+        <v>64</v>
+      </c>
+      <c r="C19">
+        <v>48</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
+      <c r="E19">
+        <v>20</v>
+      </c>
+      <c r="F19">
         <v>1</v>
       </c>
-      <c r="D2" s="4">
+      <c r="G19" t="s">
+        <v>192</v>
+      </c>
+      <c r="H19" t="s">
+        <v>203</v>
+      </c>
+      <c r="I19">
         <v>1</v>
       </c>
-      <c r="E2" s="4">
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1200</v>
+      </c>
+      <c r="B20">
+        <v>128</v>
+      </c>
+      <c r="C20">
+        <v>104</v>
+      </c>
+      <c r="D20">
+        <v>35</v>
+      </c>
+      <c r="E20">
+        <v>35</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>193</v>
+      </c>
+      <c r="H20" t="s">
+        <v>204</v>
+      </c>
+      <c r="I20">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>600</v>
+      </c>
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+      <c r="D21">
         <v>10</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21" t="s">
+        <v>194</v>
+      </c>
+      <c r="H21" t="s">
+        <v>205</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>900</v>
+      </c>
+      <c r="B22">
+        <v>96</v>
+      </c>
+      <c r="C22">
+        <v>80</v>
+      </c>
+      <c r="D22">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>25</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22" t="s">
+        <v>195</v>
+      </c>
+      <c r="H22" t="s">
+        <v>206</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>700</v>
+      </c>
+      <c r="B23">
+        <v>48</v>
+      </c>
+      <c r="C23">
         <v>36</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>50</v>
-      </c>
-      <c r="B3" s="4">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>70</v>
-      </c>
-      <c r="B4" s="4">
-        <v>16</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="D23">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <v>15</v>
+      </c>
+      <c r="F23">
         <v>5</v>
       </c>
-      <c r="D4" s="4">
-        <v>3</v>
-      </c>
-      <c r="E4" s="4">
-        <v>3</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>77</v>
-      </c>
-      <c r="B5" s="4">
-        <v>20</v>
-      </c>
-      <c r="C5" s="4">
-        <v>5</v>
-      </c>
-      <c r="D5" s="4">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4">
-        <v>4</v>
-      </c>
-      <c r="F5" s="4" t="s">
+      <c r="G23" t="s">
+        <v>196</v>
+      </c>
+      <c r="H23" t="s">
+        <v>207</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1100</v>
+      </c>
+      <c r="B24">
+        <v>120</v>
+      </c>
+      <c r="C24">
+        <v>96</v>
+      </c>
+      <c r="D24">
         <v>30</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>140</v>
-      </c>
-      <c r="B6" s="4">
+      <c r="E24">
+        <v>30</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24" t="s">
+        <v>197</v>
+      </c>
+      <c r="H24" t="s">
+        <v>208</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1000</v>
+      </c>
+      <c r="B25">
+        <v>112</v>
+      </c>
+      <c r="C25">
+        <v>92</v>
+      </c>
+      <c r="D25">
         <v>28</v>
       </c>
-      <c r="C6" s="4">
+      <c r="E25">
+        <v>28</v>
+      </c>
+      <c r="F25">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>198</v>
+      </c>
+      <c r="H25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1300</v>
+      </c>
+      <c r="B26">
+        <v>176</v>
+      </c>
+      <c r="C26">
+        <v>144</v>
+      </c>
+      <c r="D26">
+        <v>40</v>
+      </c>
+      <c r="E26">
+        <v>40</v>
+      </c>
+      <c r="F26">
         <v>8</v>
       </c>
-      <c r="D6" s="4">
-        <v>5</v>
-      </c>
-      <c r="E6" s="4">
-        <v>5</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="G26" t="s">
+        <v>199</v>
+      </c>
+      <c r="H26" t="s">
+        <v>210</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>105</v>
-      </c>
-      <c r="B7" s="4">
-        <v>32</v>
-      </c>
-      <c r="C7" s="4">
-        <v>16</v>
-      </c>
-      <c r="D7" s="4">
-        <v>8</v>
-      </c>
-      <c r="E7" s="4">
-        <v>6</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>90</v>
-      </c>
-      <c r="B8" s="4">
+      <c r="K26">
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="C8" s="4">
-        <v>28</v>
-      </c>
-      <c r="D8" s="4">
-        <v>10</v>
-      </c>
-      <c r="E8" s="4">
-        <v>7</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>105</v>
-      </c>
-      <c r="B9" s="4">
-        <v>52</v>
-      </c>
-      <c r="C9" s="4">
-        <v>24</v>
-      </c>
-      <c r="D9" s="4">
-        <v>10</v>
-      </c>
-      <c r="E9" s="4">
-        <v>8</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>210</v>
-      </c>
-      <c r="B10" s="4">
-        <v>60</v>
-      </c>
-      <c r="C10" s="4">
-        <v>36</v>
-      </c>
-      <c r="D10" s="4">
-        <v>13</v>
-      </c>
-      <c r="E10" s="4">
-        <v>10</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>280</v>
-      </c>
-      <c r="B11" s="4">
-        <v>72</v>
-      </c>
-      <c r="C11" s="4">
-        <v>40</v>
-      </c>
-      <c r="D11" s="4">
-        <v>15</v>
-      </c>
-      <c r="E11" s="4">
-        <v>12</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>350</v>
-      </c>
-      <c r="B12" s="4">
-        <v>92</v>
-      </c>
-      <c r="C12" s="4">
-        <v>52</v>
-      </c>
-      <c r="D12" s="4">
-        <v>15</v>
-      </c>
-      <c r="E12" s="4">
-        <v>15</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>175</v>
-      </c>
-      <c r="B13" s="4">
-        <v>96</v>
-      </c>
-      <c r="C13" s="4">
-        <v>56</v>
-      </c>
-      <c r="D13" s="4">
-        <v>20</v>
-      </c>
-      <c r="E13" s="4">
-        <v>17</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>315</v>
-      </c>
-      <c r="B14" s="4">
+    </row>
+    <row r="27" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2500</v>
+      </c>
+      <c r="B27">
         <v>120</v>
       </c>
-      <c r="C14" s="4">
-        <v>72</v>
-      </c>
-      <c r="D14" s="4">
-        <v>22</v>
-      </c>
-      <c r="E14" s="4">
-        <v>19</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>385</v>
-      </c>
-      <c r="B15" s="4">
-        <v>128</v>
-      </c>
-      <c r="C15" s="4">
-        <v>72</v>
-      </c>
-      <c r="D15" s="4">
-        <v>25</v>
-      </c>
-      <c r="E15" s="4">
-        <v>20</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>70</v>
-      </c>
-      <c r="B16" s="4">
-        <v>160</v>
-      </c>
-      <c r="C16" s="4">
-        <v>88</v>
-      </c>
-      <c r="D16" s="4">
-        <v>30</v>
-      </c>
-      <c r="E16" s="4">
-        <v>25</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>490</v>
-      </c>
-      <c r="B17" s="4">
-        <v>168</v>
-      </c>
-      <c r="C17" s="4">
-        <v>100</v>
-      </c>
-      <c r="D17" s="4">
-        <v>32</v>
-      </c>
-      <c r="E17" s="4">
-        <v>30</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>910</v>
-      </c>
-      <c r="B18" s="4">
-        <v>192</v>
-      </c>
-      <c r="C18" s="4">
-        <v>100</v>
-      </c>
-      <c r="D18" s="4">
-        <v>40</v>
-      </c>
-      <c r="E18" s="4">
-        <v>35</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>560</v>
-      </c>
-      <c r="B19" s="4">
-        <v>48</v>
-      </c>
-      <c r="C19" s="4">
-        <v>40</v>
-      </c>
-      <c r="D19" s="4">
-        <v>60</v>
-      </c>
-      <c r="E19" s="4">
-        <v>60</v>
-      </c>
-      <c r="F19" s="4">
-        <v>1</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>840</v>
-      </c>
-      <c r="B20" s="4">
-        <v>104</v>
-      </c>
-      <c r="C20" s="4">
-        <v>72</v>
-      </c>
-      <c r="D20" s="4">
+      <c r="C27">
         <v>80</v>
       </c>
-      <c r="E20" s="4">
-        <v>80</v>
-      </c>
-      <c r="F20" s="4">
-        <v>2</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>420</v>
-      </c>
-      <c r="B21" s="4">
-        <v>18</v>
-      </c>
-      <c r="C21" s="4">
-        <v>12</v>
-      </c>
-      <c r="D21" s="4">
-        <v>50</v>
-      </c>
-      <c r="E21" s="4">
-        <v>50</v>
-      </c>
-      <c r="F21" s="4">
-        <v>3</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>630</v>
-      </c>
-      <c r="B22" s="4">
-        <v>56</v>
-      </c>
-      <c r="C22" s="4">
-        <v>48</v>
-      </c>
-      <c r="D22" s="4">
-        <v>65</v>
-      </c>
-      <c r="E22" s="4">
-        <v>65</v>
-      </c>
-      <c r="F22" s="4">
-        <v>4</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>490</v>
-      </c>
-      <c r="B23" s="4">
-        <v>28</v>
-      </c>
-      <c r="C23" s="4">
-        <v>24</v>
-      </c>
-      <c r="D23" s="4">
-        <v>55</v>
-      </c>
-      <c r="E23" s="4">
-        <v>55</v>
-      </c>
-      <c r="F23" s="4">
-        <v>5</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>770</v>
-      </c>
-      <c r="B24" s="4">
-        <v>96</v>
-      </c>
-      <c r="C24" s="4">
-        <v>64</v>
-      </c>
-      <c r="D24" s="4">
+      <c r="D27">
+        <v>84</v>
+      </c>
+      <c r="E27">
         <v>75</v>
       </c>
-      <c r="E24" s="4">
-        <v>75</v>
-      </c>
-      <c r="F24" s="4">
-        <v>6</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>700</v>
-      </c>
-      <c r="B25" s="4">
-        <v>72</v>
-      </c>
-      <c r="C25" s="4">
-        <v>48</v>
-      </c>
-      <c r="D25" s="4">
-        <v>70</v>
-      </c>
-      <c r="E25" s="4">
-        <v>70</v>
-      </c>
-      <c r="F25" s="4">
-        <v>7</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>910</v>
-      </c>
-      <c r="B26" s="4">
-        <v>120</v>
-      </c>
-      <c r="C26" s="4">
-        <v>80</v>
-      </c>
-      <c r="D26" s="4">
-        <v>85</v>
-      </c>
-      <c r="E26" s="4">
-        <v>85</v>
-      </c>
-      <c r="F26" s="4">
-        <v>8</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>1750</v>
-      </c>
-      <c r="B27" s="4">
-        <v>480</v>
-      </c>
-      <c r="C27" s="4">
-        <v>400</v>
-      </c>
-      <c r="D27" s="4">
-        <v>84</v>
-      </c>
-      <c r="E27" s="4">
-        <v>75</v>
-      </c>
-      <c r="G27" s="4" t="s">
+      <c r="F27"/>
+      <c r="G27" t="s">
         <v>212</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>2100</v>
-      </c>
-      <c r="B28" s="4">
-        <v>640</v>
-      </c>
-      <c r="C28" s="4">
-        <v>560</v>
-      </c>
-      <c r="D28" s="4">
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+    </row>
+    <row r="28" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3000</v>
+      </c>
+      <c r="B28">
+        <v>200</v>
+      </c>
+      <c r="C28">
+        <v>150</v>
+      </c>
+      <c r="D28">
         <v>250</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28">
         <v>220</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="F28"/>
+      <c r="G28" t="s">
         <v>143</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
         <v>68</v>
       </c>
@@ -5038,10 +5730,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -5053,10 +5745,10 @@
     <col min="5" max="5" width="5.796875" customWidth="1"/>
     <col min="6" max="6" width="8.59765625" customWidth="1"/>
     <col min="9" max="9" width="6.796875" customWidth="1"/>
-    <col min="10" max="10" width="5.69921875" customWidth="1"/>
+    <col min="10" max="10" width="7.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -5075,22 +5767,31 @@
       <c r="F1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J1" t="s">
+        <v>218</v>
+      </c>
+      <c r="K1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B2">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -5101,22 +5802,33 @@
       <c r="H2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <f>I2*E2</f>
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <f>I2*D2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
       <c r="E3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
         <v>26</v>
@@ -5127,22 +5839,33 @@
       <c r="H3" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J26" si="0">I3*E3</f>
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K26" si="1">I3*D3</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B4">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>
@@ -5153,22 +5876,33 @@
       <c r="H4" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>15</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
         <v>5</v>
       </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
       <c r="E5">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
         <v>30</v>
@@ -5179,22 +5913,33 @@
       <c r="H5" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="B6">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F6" t="s">
         <v>32</v>
@@ -5205,22 +5950,33 @@
       <c r="H6" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="B7">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D7">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E7">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F7" t="s">
         <v>33</v>
@@ -5231,22 +5987,33 @@
       <c r="H7" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B8">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C8">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E8">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
         <v>34</v>
@@ -5257,22 +6024,33 @@
       <c r="H8" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="B9">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C9">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D9">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E9">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
         <v>35</v>
@@ -5283,22 +6061,33 @@
       <c r="H9" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>9</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="B10">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="C10">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D10">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E10">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
         <v>53</v>
@@ -5309,22 +6098,33 @@
       <c r="H10" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>280</v>
+        <v>320</v>
       </c>
       <c r="B11">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="C11">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E11">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
         <v>54</v>
@@ -5335,22 +6135,33 @@
       <c r="H11" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="B12">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="C12">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D12">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E12">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F12" t="s">
         <v>55</v>
@@ -5361,22 +6172,33 @@
       <c r="H12" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="B13">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="C13">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D13">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E13">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
         <v>56</v>
@@ -5387,22 +6209,33 @@
       <c r="H13" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>315</v>
+        <v>360</v>
       </c>
       <c r="B14">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="C14">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="D14">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E14">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F14" t="s">
         <v>57</v>
@@ -5413,22 +6246,33 @@
       <c r="H14" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>385</v>
+        <v>440</v>
       </c>
       <c r="B15">
-        <v>128</v>
+        <v>65</v>
       </c>
       <c r="C15">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D15">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E15">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F15" t="s">
         <v>58</v>
@@ -5439,22 +6283,33 @@
       <c r="H15" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>70</v>
+        <v>480</v>
       </c>
       <c r="B16">
-        <v>160</v>
+        <v>68</v>
       </c>
       <c r="C16">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="D16">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E16">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F16" t="s">
         <v>59</v>
@@ -5465,22 +6320,33 @@
       <c r="H16" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>490</v>
+        <v>560</v>
       </c>
       <c r="B17">
-        <v>168</v>
+        <v>70</v>
       </c>
       <c r="C17">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="D17">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E17">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F17" t="s">
         <v>60</v>
@@ -5491,22 +6357,33 @@
       <c r="H17" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>910</v>
+        <v>1040</v>
       </c>
       <c r="B18">
-        <v>192</v>
+        <v>65</v>
       </c>
       <c r="C18">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D18">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="E18">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="F18" t="s">
         <v>61</v>
@@ -5517,22 +6394,33 @@
       <c r="H18" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>7</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>154</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>560</v>
+        <v>640</v>
       </c>
       <c r="B19">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C19">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D19">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="E19">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -5543,22 +6431,33 @@
       <c r="H19" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>840</v>
+        <v>960</v>
       </c>
       <c r="B20">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C20">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D20">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="E20">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="F20">
         <v>2</v>
@@ -5569,22 +6468,33 @@
       <c r="H20" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="B21">
-        <v>17.600000000000001</v>
+        <v>11</v>
       </c>
       <c r="C21">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D21">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E21">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="F21">
         <v>3</v>
@@ -5595,22 +6505,33 @@
       <c r="H21" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>630</v>
+        <v>720</v>
       </c>
       <c r="B22">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C22">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D22">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="E22">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="F22">
         <v>4</v>
@@ -5621,22 +6542,33 @@
       <c r="H22" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>490</v>
+        <v>560</v>
       </c>
       <c r="B23">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C23">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D23">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="E23">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="F23">
         <v>5</v>
@@ -5647,22 +6579,33 @@
       <c r="H23" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>770</v>
+        <v>880</v>
       </c>
       <c r="B24">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="C24">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D24">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="E24">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="F24">
         <v>6</v>
@@ -5673,22 +6616,33 @@
       <c r="H24" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="B25">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C25">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="D25">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="E25">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="F25">
         <v>7</v>
@@ -5699,22 +6653,33 @@
       <c r="H25" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>910</v>
+        <v>1040</v>
       </c>
       <c r="B26">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C26">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="D26">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="E26">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="F26">
         <v>8</v>
@@ -5725,22 +6690,33 @@
       <c r="H26" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>1750</v>
+        <v>2000</v>
       </c>
       <c r="B27">
-        <v>480</v>
+        <v>120</v>
       </c>
       <c r="C27">
-        <v>400</v>
+        <v>80</v>
       </c>
       <c r="D27">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E27">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G27" t="s">
         <v>212</v>
@@ -5749,21 +6725,21 @@
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2100</v>
+        <v>2400</v>
       </c>
       <c r="B28">
-        <v>640</v>
+        <v>140</v>
       </c>
       <c r="C28">
-        <v>560</v>
+        <v>100</v>
       </c>
       <c r="D28">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E28">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G28" t="s">
         <v>143</v>
@@ -5772,7 +6748,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
         <v>68</v>
       </c>
@@ -5829,7 +6805,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -6215,7 +7191,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -6823,7 +7799,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -7458,7 +8434,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -8042,7 +9018,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -8670,7 +9646,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>

</xml_diff>